<commit_message>
Hydroethanolic extract R Script.
</commit_message>
<xml_diff>
--- a/Data/Antimicrobial_H2O.xlsx
+++ b/Data/Antimicrobial_H2O.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F4ss0\Documents\Ikiam21062022\Proyecto Guayusa\Antimicrobial_I_guayusa\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65BBF08-B4F2-4254-B6C0-DF7488152F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F38CE5-C19E-48C3-BE9D-EE27B65FE99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AE241DF6-4FFC-4DF2-B60A-123CF49BB9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Escalas" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51317C54-FA6A-412C-98DB-C8D1CBD7C6B3}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2585,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8542F08-6268-4576-8880-7C096C0A263D}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>